<commit_message>
Updated datasheet to exclude column that was not used in the analyses
</commit_message>
<xml_diff>
--- a/eABS_property_data_JCIM.xlsx
+++ b/eABS_property_data_JCIM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-repositories\eABS_data_JCIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5410E088-1BE9-44A4-A3CD-B977DA4C3FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24F385D-CACC-4E69-AC94-32AF1D336B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6439F25F-76EA-4B7C-82CE-F7B7B679C2EA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="714">
   <si>
     <t>Sample</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Charpy Impact</t>
   </si>
   <si>
-    <t>Pendulum Charpy</t>
-  </si>
-  <si>
     <t>Displacement to Peak</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>5.75</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>4.43</t>
   </si>
   <si>
@@ -241,9 +235,6 @@
     <t>12.70</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>8.92</t>
   </si>
   <si>
@@ -293,9 +284,6 @@
   </si>
   <si>
     <t>15.91</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
   <si>
     <t>18.72</t>
@@ -2586,10 +2574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D2A639-30E7-49EF-B70E-774C650BC2EF}">
-  <dimension ref="A1:T43"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2603,27 +2591,26 @@
     <col min="10" max="10" width="29" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>709</v>
+      </c>
+      <c r="C1" t="s">
         <v>713</v>
       </c>
-      <c r="C1" t="s">
-        <v>717</v>
-      </c>
       <c r="D1" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2650,13 +2637,13 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
+        <v>710</v>
+      </c>
+      <c r="N1" t="s">
+        <v>711</v>
+      </c>
+      <c r="O1" t="s">
         <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>714</v>
-      </c>
-      <c r="O1" t="s">
-        <v>715</v>
       </c>
       <c r="P1" t="s">
         <v>11</v>
@@ -2670,13 +2657,10 @@
       <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
       </c>
       <c r="B2">
         <v>17</v>
@@ -2685,60 +2669,57 @@
         <v>48.5</v>
       </c>
       <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
       <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
       </c>
       <c r="M2" t="s">
         <v>29</v>
       </c>
       <c r="N2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" t="s">
         <v>31</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>32</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>34</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>35</v>
       </c>
-      <c r="S2" t="s">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -2747,60 +2728,57 @@
         <v>48.3</v>
       </c>
       <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
         <v>39</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>40</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>41</v>
       </c>
-      <c r="G3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
       <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s">
         <v>46</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>47</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>48</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>49</v>
       </c>
-      <c r="M3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>50</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>51</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>53</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>54</v>
       </c>
-      <c r="S3" t="s">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>55</v>
-      </c>
-      <c r="T3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>57</v>
       </c>
       <c r="B4">
         <v>23</v>
@@ -2809,60 +2787,57 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
         <v>58</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
         <v>59</v>
       </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>61</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" t="s">
         <v>63</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>64</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>65</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>66</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>67</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>68</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>69</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>70</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>71</v>
       </c>
-      <c r="R4" t="s">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>72</v>
-      </c>
-      <c r="S4" t="s">
-        <v>73</v>
-      </c>
-      <c r="T4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>75</v>
       </c>
       <c r="B5">
         <v>26</v>
@@ -2871,60 +2846,57 @@
         <v>48.4</v>
       </c>
       <c r="D5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" t="s">
         <v>76</v>
       </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>79</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5" t="s">
         <v>82</v>
       </c>
-      <c r="J5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>83</v>
       </c>
-      <c r="L5" t="s">
+      <c r="O5" t="s">
         <v>84</v>
       </c>
-      <c r="M5" t="s">
+      <c r="P5" t="s">
         <v>85</v>
       </c>
-      <c r="N5" t="s">
+      <c r="Q5" t="s">
         <v>86</v>
       </c>
-      <c r="O5" t="s">
+      <c r="R5" t="s">
         <v>87</v>
       </c>
-      <c r="P5" t="s">
+      <c r="S5" t="s">
         <v>88</v>
       </c>
-      <c r="Q5" t="s">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>89</v>
-      </c>
-      <c r="R5" t="s">
-        <v>90</v>
-      </c>
-      <c r="S5" t="s">
-        <v>91</v>
-      </c>
-      <c r="T5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>93</v>
       </c>
       <c r="B6">
         <v>29</v>
@@ -2933,60 +2905,57 @@
         <v>48.5</v>
       </c>
       <c r="D6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" t="s">
         <v>94</v>
       </c>
-      <c r="E6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
         <v>96</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
         <v>97</v>
       </c>
-      <c r="H6" t="s">
+      <c r="L6" t="s">
         <v>98</v>
       </c>
-      <c r="I6" t="s">
+      <c r="M6" t="s">
+        <v>99</v>
+      </c>
+      <c r="N6" t="s">
         <v>100</v>
       </c>
-      <c r="J6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="O6" t="s">
         <v>101</v>
       </c>
-      <c r="L6" t="s">
+      <c r="P6" t="s">
         <v>102</v>
       </c>
-      <c r="M6" t="s">
-        <v>85</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="Q6" t="s">
         <v>103</v>
       </c>
-      <c r="O6" t="s">
+      <c r="R6" t="s">
         <v>104</v>
       </c>
-      <c r="P6" t="s">
+      <c r="S6" t="s">
         <v>105</v>
       </c>
-      <c r="Q6" t="s">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>106</v>
-      </c>
-      <c r="R6" t="s">
-        <v>107</v>
-      </c>
-      <c r="S6" t="s">
-        <v>108</v>
-      </c>
-      <c r="T6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>110</v>
       </c>
       <c r="B7">
         <v>32</v>
@@ -2995,60 +2964,57 @@
         <v>48.1</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" t="s">
         <v>113</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>114</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L7" t="s">
+        <v>116</v>
+      </c>
+      <c r="M7" t="s">
         <v>117</v>
       </c>
-      <c r="J7" t="s">
+      <c r="N7" t="s">
         <v>118</v>
       </c>
-      <c r="K7" t="s">
+      <c r="O7" t="s">
         <v>119</v>
       </c>
-      <c r="L7" t="s">
+      <c r="P7" t="s">
         <v>120</v>
       </c>
-      <c r="M7" t="s">
-        <v>85</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="Q7" t="s">
         <v>121</v>
       </c>
-      <c r="O7" t="s">
+      <c r="R7" t="s">
         <v>122</v>
       </c>
-      <c r="P7" t="s">
+      <c r="S7" t="s">
         <v>123</v>
       </c>
-      <c r="Q7" t="s">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>124</v>
-      </c>
-      <c r="R7" t="s">
-        <v>125</v>
-      </c>
-      <c r="S7" t="s">
-        <v>126</v>
-      </c>
-      <c r="T7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>128</v>
       </c>
       <c r="B8">
         <v>35</v>
@@ -3057,60 +3023,57 @@
         <v>48.3</v>
       </c>
       <c r="D8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" t="s">
         <v>129</v>
       </c>
-      <c r="E8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="I8" t="s">
         <v>131</v>
       </c>
-      <c r="G8" t="s">
+      <c r="J8" t="s">
         <v>132</v>
       </c>
-      <c r="H8" t="s">
+      <c r="K8" t="s">
         <v>133</v>
       </c>
-      <c r="I8" t="s">
+      <c r="L8" t="s">
+        <v>134</v>
+      </c>
+      <c r="M8" t="s">
         <v>135</v>
       </c>
-      <c r="J8" t="s">
+      <c r="N8" t="s">
         <v>136</v>
       </c>
-      <c r="K8" t="s">
+      <c r="O8" t="s">
         <v>137</v>
       </c>
-      <c r="L8" t="s">
+      <c r="P8" t="s">
         <v>138</v>
       </c>
-      <c r="M8" t="s">
-        <v>67</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="Q8" t="s">
         <v>139</v>
       </c>
-      <c r="O8" t="s">
+      <c r="R8" t="s">
         <v>140</v>
       </c>
-      <c r="P8" t="s">
+      <c r="S8" t="s">
         <v>141</v>
       </c>
-      <c r="Q8" t="s">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>142</v>
-      </c>
-      <c r="R8" t="s">
-        <v>143</v>
-      </c>
-      <c r="S8" t="s">
-        <v>144</v>
-      </c>
-      <c r="T8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>146</v>
       </c>
       <c r="B9">
         <v>17</v>
@@ -3119,60 +3082,57 @@
         <v>50.9</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H9" t="s">
+        <v>146</v>
+      </c>
+      <c r="I9" t="s">
         <v>148</v>
       </c>
-      <c r="G9" t="s">
+      <c r="J9" t="s">
         <v>149</v>
       </c>
-      <c r="H9" t="s">
+      <c r="K9" t="s">
         <v>150</v>
       </c>
-      <c r="I9" t="s">
+      <c r="L9" t="s">
+        <v>151</v>
+      </c>
+      <c r="M9" t="s">
         <v>152</v>
       </c>
-      <c r="J9" t="s">
+      <c r="N9" t="s">
         <v>153</v>
       </c>
-      <c r="K9" t="s">
+      <c r="O9" t="s">
         <v>154</v>
       </c>
-      <c r="L9" t="s">
+      <c r="P9" t="s">
         <v>155</v>
       </c>
-      <c r="M9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="Q9" t="s">
         <v>156</v>
       </c>
-      <c r="O9" t="s">
+      <c r="R9" t="s">
         <v>157</v>
       </c>
-      <c r="P9" t="s">
+      <c r="S9" t="s">
         <v>158</v>
       </c>
-      <c r="Q9" t="s">
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>159</v>
-      </c>
-      <c r="R9" t="s">
-        <v>160</v>
-      </c>
-      <c r="S9" t="s">
-        <v>161</v>
-      </c>
-      <c r="T9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>163</v>
       </c>
       <c r="B10">
         <v>20</v>
@@ -3181,60 +3141,57 @@
         <v>50.9</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
+        <v>161</v>
+      </c>
+      <c r="G10" t="s">
+        <v>162</v>
+      </c>
+      <c r="H10" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" t="s">
         <v>165</v>
       </c>
-      <c r="G10" t="s">
+      <c r="J10" t="s">
         <v>166</v>
       </c>
-      <c r="H10" t="s">
+      <c r="K10" t="s">
         <v>167</v>
       </c>
-      <c r="I10" t="s">
+      <c r="L10" t="s">
+        <v>168</v>
+      </c>
+      <c r="M10" t="s">
         <v>169</v>
       </c>
-      <c r="J10" t="s">
+      <c r="N10" t="s">
         <v>170</v>
       </c>
-      <c r="K10" t="s">
+      <c r="O10" t="s">
         <v>171</v>
       </c>
-      <c r="L10" t="s">
+      <c r="P10" t="s">
         <v>172</v>
       </c>
-      <c r="M10" t="s">
-        <v>29</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="Q10" t="s">
         <v>173</v>
       </c>
-      <c r="O10" t="s">
+      <c r="R10" t="s">
         <v>174</v>
       </c>
-      <c r="P10" t="s">
+      <c r="S10" t="s">
         <v>175</v>
       </c>
-      <c r="Q10" t="s">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>176</v>
-      </c>
-      <c r="R10" t="s">
-        <v>177</v>
-      </c>
-      <c r="S10" t="s">
-        <v>178</v>
-      </c>
-      <c r="T10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>180</v>
       </c>
       <c r="B11">
         <v>23</v>
@@ -3243,60 +3200,57 @@
         <v>50.8</v>
       </c>
       <c r="D11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F11" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G11" t="s">
+        <v>179</v>
+      </c>
+      <c r="H11" t="s">
+        <v>180</v>
+      </c>
+      <c r="I11" t="s">
         <v>183</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>184</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
+        <v>185</v>
+      </c>
+      <c r="L11" t="s">
+        <v>186</v>
+      </c>
+      <c r="M11" t="s">
         <v>187</v>
       </c>
-      <c r="J11" t="s">
+      <c r="N11" t="s">
         <v>188</v>
       </c>
-      <c r="K11" t="s">
+      <c r="O11" t="s">
         <v>189</v>
       </c>
-      <c r="L11" t="s">
+      <c r="P11" t="s">
         <v>190</v>
       </c>
-      <c r="M11" t="s">
-        <v>67</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="Q11" t="s">
         <v>191</v>
       </c>
-      <c r="O11" t="s">
+      <c r="R11" t="s">
         <v>192</v>
       </c>
-      <c r="P11" t="s">
+      <c r="S11" t="s">
         <v>193</v>
       </c>
-      <c r="Q11" t="s">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>194</v>
-      </c>
-      <c r="R11" t="s">
-        <v>195</v>
-      </c>
-      <c r="S11" t="s">
-        <v>196</v>
-      </c>
-      <c r="T11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>198</v>
       </c>
       <c r="B12">
         <v>26</v>
@@ -3305,60 +3259,57 @@
         <v>51.1</v>
       </c>
       <c r="D12" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E12" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F12" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G12" t="s">
+        <v>197</v>
+      </c>
+      <c r="H12" t="s">
+        <v>198</v>
+      </c>
+      <c r="I12" t="s">
         <v>201</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>202</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
+        <v>203</v>
+      </c>
+      <c r="L12" t="s">
+        <v>204</v>
+      </c>
+      <c r="M12" t="s">
         <v>205</v>
       </c>
-      <c r="J12" t="s">
+      <c r="N12" t="s">
         <v>206</v>
       </c>
-      <c r="K12" t="s">
+      <c r="O12" t="s">
         <v>207</v>
       </c>
-      <c r="L12" t="s">
+      <c r="P12" t="s">
         <v>208</v>
       </c>
-      <c r="M12" t="s">
-        <v>67</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="Q12" t="s">
         <v>209</v>
       </c>
-      <c r="O12" t="s">
+      <c r="R12" t="s">
         <v>210</v>
       </c>
-      <c r="P12" t="s">
+      <c r="S12" t="s">
         <v>211</v>
       </c>
-      <c r="Q12" t="s">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>212</v>
-      </c>
-      <c r="R12" t="s">
-        <v>213</v>
-      </c>
-      <c r="S12" t="s">
-        <v>214</v>
-      </c>
-      <c r="T12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>216</v>
       </c>
       <c r="B13">
         <v>29</v>
@@ -3367,60 +3318,57 @@
         <v>51.3</v>
       </c>
       <c r="D13" t="s">
+        <v>213</v>
+      </c>
+      <c r="E13" t="s">
+        <v>214</v>
+      </c>
+      <c r="F13" t="s">
+        <v>215</v>
+      </c>
+      <c r="G13" t="s">
+        <v>216</v>
+      </c>
+      <c r="H13" t="s">
         <v>217</v>
       </c>
-      <c r="E13" t="s">
-        <v>218</v>
-      </c>
-      <c r="F13" t="s">
-        <v>219</v>
-      </c>
-      <c r="G13" t="s">
-        <v>220</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>221</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
+        <v>222</v>
+      </c>
+      <c r="K13" t="s">
+        <v>223</v>
+      </c>
+      <c r="L13" t="s">
+        <v>224</v>
+      </c>
+      <c r="M13" t="s">
         <v>225</v>
       </c>
-      <c r="J13" t="s">
+      <c r="N13" t="s">
         <v>226</v>
       </c>
-      <c r="K13" t="s">
+      <c r="O13" t="s">
         <v>227</v>
       </c>
-      <c r="L13" t="s">
+      <c r="P13" t="s">
         <v>228</v>
       </c>
-      <c r="M13" t="s">
-        <v>85</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="Q13" t="s">
         <v>229</v>
       </c>
-      <c r="O13" t="s">
+      <c r="R13" t="s">
         <v>230</v>
       </c>
-      <c r="P13" t="s">
+      <c r="S13" t="s">
         <v>231</v>
       </c>
-      <c r="Q13" t="s">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>232</v>
-      </c>
-      <c r="R13" t="s">
-        <v>233</v>
-      </c>
-      <c r="S13" t="s">
-        <v>234</v>
-      </c>
-      <c r="T13" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>236</v>
       </c>
       <c r="B14">
         <v>32</v>
@@ -3429,60 +3377,57 @@
         <v>51.4</v>
       </c>
       <c r="D14" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G14" t="s">
+        <v>235</v>
+      </c>
+      <c r="H14" t="s">
+        <v>236</v>
+      </c>
+      <c r="I14" t="s">
         <v>238</v>
       </c>
-      <c r="G14" t="s">
+      <c r="J14" t="s">
         <v>239</v>
       </c>
-      <c r="H14" t="s">
+      <c r="K14" t="s">
         <v>240</v>
       </c>
-      <c r="I14" t="s">
-        <v>242</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
+        <v>241</v>
+      </c>
+      <c r="M14" t="s">
         <v>243</v>
       </c>
-      <c r="K14" t="s">
+      <c r="N14" t="s">
         <v>244</v>
       </c>
-      <c r="L14" t="s">
+      <c r="O14" t="s">
         <v>245</v>
       </c>
-      <c r="M14" t="s">
-        <v>85</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="P14" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q14" t="s">
         <v>247</v>
       </c>
-      <c r="O14" t="s">
+      <c r="R14" t="s">
         <v>248</v>
       </c>
-      <c r="P14" t="s">
+      <c r="S14" t="s">
         <v>249</v>
       </c>
-      <c r="Q14" t="s">
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>250</v>
-      </c>
-      <c r="R14" t="s">
-        <v>251</v>
-      </c>
-      <c r="S14" t="s">
-        <v>252</v>
-      </c>
-      <c r="T14" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>254</v>
       </c>
       <c r="B15">
         <v>35</v>
@@ -3491,60 +3436,57 @@
         <v>51.1</v>
       </c>
       <c r="D15" t="s">
+        <v>251</v>
+      </c>
+      <c r="E15" t="s">
+        <v>252</v>
+      </c>
+      <c r="F15" t="s">
+        <v>253</v>
+      </c>
+      <c r="G15" t="s">
+        <v>254</v>
+      </c>
+      <c r="H15" t="s">
         <v>255</v>
       </c>
-      <c r="E15" t="s">
-        <v>256</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>257</v>
       </c>
-      <c r="G15" t="s">
+      <c r="J15" t="s">
         <v>258</v>
       </c>
-      <c r="H15" t="s">
+      <c r="K15" t="s">
         <v>259</v>
       </c>
-      <c r="I15" t="s">
-        <v>261</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
+        <v>260</v>
+      </c>
+      <c r="M15" t="s">
         <v>262</v>
       </c>
-      <c r="K15" t="s">
+      <c r="N15" t="s">
         <v>263</v>
       </c>
-      <c r="L15" t="s">
+      <c r="O15" t="s">
         <v>264</v>
       </c>
-      <c r="M15" t="s">
-        <v>85</v>
-      </c>
-      <c r="N15" t="s">
+      <c r="P15" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q15" t="s">
         <v>266</v>
       </c>
-      <c r="O15" t="s">
+      <c r="R15" t="s">
         <v>267</v>
       </c>
-      <c r="P15" t="s">
+      <c r="S15" t="s">
         <v>268</v>
       </c>
-      <c r="Q15" t="s">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>269</v>
-      </c>
-      <c r="R15" t="s">
-        <v>270</v>
-      </c>
-      <c r="S15" t="s">
-        <v>271</v>
-      </c>
-      <c r="T15" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>273</v>
       </c>
       <c r="B16">
         <v>17</v>
@@ -3553,60 +3495,57 @@
         <v>61.4</v>
       </c>
       <c r="D16" t="s">
+        <v>270</v>
+      </c>
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>271</v>
+      </c>
+      <c r="G16" t="s">
+        <v>272</v>
+      </c>
+      <c r="H16" t="s">
+        <v>273</v>
+      </c>
+      <c r="I16" t="s">
         <v>274</v>
       </c>
-      <c r="E16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="J16" t="s">
+        <v>132</v>
+      </c>
+      <c r="K16" t="s">
         <v>275</v>
       </c>
-      <c r="G16" t="s">
+      <c r="L16" t="s">
         <v>276</v>
       </c>
-      <c r="H16" t="s">
+      <c r="M16" t="s">
         <v>277</v>
       </c>
-      <c r="I16" t="s">
+      <c r="N16" t="s">
         <v>278</v>
       </c>
-      <c r="J16" t="s">
-        <v>136</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="O16" t="s">
+        <v>47</v>
+      </c>
+      <c r="P16" t="s">
         <v>279</v>
       </c>
-      <c r="L16" t="s">
+      <c r="Q16" t="s">
         <v>280</v>
       </c>
-      <c r="M16" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" t="s">
+      <c r="R16" t="s">
         <v>281</v>
       </c>
-      <c r="O16" t="s">
+      <c r="S16" t="s">
         <v>282</v>
       </c>
-      <c r="P16" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q16" t="s">
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>283</v>
-      </c>
-      <c r="R16" t="s">
-        <v>284</v>
-      </c>
-      <c r="S16" t="s">
-        <v>285</v>
-      </c>
-      <c r="T16" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>287</v>
       </c>
       <c r="B17">
         <v>20</v>
@@ -3615,60 +3554,57 @@
         <v>61.2</v>
       </c>
       <c r="D17" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E17" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F17" t="s">
+        <v>285</v>
+      </c>
+      <c r="G17" t="s">
+        <v>286</v>
+      </c>
+      <c r="H17" t="s">
+        <v>287</v>
+      </c>
+      <c r="I17" t="s">
         <v>289</v>
       </c>
-      <c r="G17" t="s">
+      <c r="J17" t="s">
         <v>290</v>
       </c>
-      <c r="H17" t="s">
+      <c r="K17" t="s">
         <v>291</v>
       </c>
-      <c r="I17" t="s">
+      <c r="L17" t="s">
+        <v>292</v>
+      </c>
+      <c r="M17" t="s">
         <v>293</v>
       </c>
-      <c r="J17" t="s">
+      <c r="N17" t="s">
         <v>294</v>
       </c>
-      <c r="K17" t="s">
+      <c r="O17" t="s">
         <v>295</v>
       </c>
-      <c r="L17" t="s">
+      <c r="P17" t="s">
         <v>296</v>
       </c>
-      <c r="M17" t="s">
-        <v>85</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="Q17" t="s">
         <v>297</v>
       </c>
-      <c r="O17" t="s">
+      <c r="R17" t="s">
         <v>298</v>
       </c>
-      <c r="P17" t="s">
+      <c r="S17" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>299</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>300</v>
-      </c>
-      <c r="R17" t="s">
-        <v>301</v>
-      </c>
-      <c r="S17" t="s">
-        <v>302</v>
-      </c>
-      <c r="T17" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>303</v>
       </c>
       <c r="B18">
         <v>23</v>
@@ -3677,60 +3613,57 @@
         <v>61.7</v>
       </c>
       <c r="D18" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F18" t="s">
+        <v>301</v>
+      </c>
+      <c r="G18" t="s">
+        <v>302</v>
+      </c>
+      <c r="H18" t="s">
+        <v>303</v>
+      </c>
+      <c r="I18" t="s">
         <v>305</v>
       </c>
-      <c r="G18" t="s">
+      <c r="J18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" t="s">
         <v>306</v>
       </c>
-      <c r="H18" t="s">
+      <c r="L18" t="s">
         <v>307</v>
       </c>
-      <c r="I18" t="s">
+      <c r="M18" t="s">
+        <v>308</v>
+      </c>
+      <c r="N18" t="s">
         <v>309</v>
       </c>
-      <c r="J18" t="s">
-        <v>30</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="O18" t="s">
         <v>310</v>
       </c>
-      <c r="L18" t="s">
+      <c r="P18" t="s">
         <v>311</v>
       </c>
-      <c r="M18" t="s">
-        <v>85</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="Q18" t="s">
         <v>312</v>
       </c>
-      <c r="O18" t="s">
+      <c r="R18" t="s">
         <v>313</v>
       </c>
-      <c r="P18" t="s">
+      <c r="S18" t="s">
         <v>314</v>
       </c>
-      <c r="Q18" t="s">
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>315</v>
-      </c>
-      <c r="R18" t="s">
-        <v>316</v>
-      </c>
-      <c r="S18" t="s">
-        <v>317</v>
-      </c>
-      <c r="T18" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>319</v>
       </c>
       <c r="B19">
         <v>26</v>
@@ -3739,60 +3672,57 @@
         <v>61.1</v>
       </c>
       <c r="D19" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F19" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="G19" t="s">
+        <v>318</v>
+      </c>
+      <c r="H19" t="s">
+        <v>319</v>
+      </c>
+      <c r="I19" t="s">
         <v>322</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
+        <v>184</v>
+      </c>
+      <c r="K19" t="s">
         <v>323</v>
       </c>
-      <c r="I19" t="s">
+      <c r="L19" t="s">
+        <v>324</v>
+      </c>
+      <c r="M19" t="s">
+        <v>325</v>
+      </c>
+      <c r="N19" t="s">
         <v>326</v>
       </c>
-      <c r="J19" t="s">
-        <v>188</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="O19" t="s">
         <v>327</v>
       </c>
-      <c r="L19" t="s">
+      <c r="P19" t="s">
         <v>328</v>
       </c>
-      <c r="M19" t="s">
-        <v>85</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="Q19" t="s">
         <v>329</v>
       </c>
-      <c r="O19" t="s">
+      <c r="R19" t="s">
         <v>330</v>
       </c>
-      <c r="P19" t="s">
+      <c r="S19" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>331</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>332</v>
-      </c>
-      <c r="R19" t="s">
-        <v>333</v>
-      </c>
-      <c r="S19" t="s">
-        <v>334</v>
-      </c>
-      <c r="T19" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>335</v>
       </c>
       <c r="B20">
         <v>29</v>
@@ -3801,60 +3731,57 @@
         <v>61.1</v>
       </c>
       <c r="D20" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E20" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F20" t="s">
+        <v>333</v>
+      </c>
+      <c r="G20" t="s">
+        <v>334</v>
+      </c>
+      <c r="H20" t="s">
+        <v>335</v>
+      </c>
+      <c r="I20" t="s">
         <v>337</v>
       </c>
-      <c r="G20" t="s">
+      <c r="J20" t="s">
         <v>338</v>
       </c>
-      <c r="H20" t="s">
+      <c r="K20" t="s">
         <v>339</v>
       </c>
-      <c r="I20" t="s">
+      <c r="L20" t="s">
+        <v>340</v>
+      </c>
+      <c r="M20" t="s">
         <v>341</v>
       </c>
-      <c r="J20" t="s">
+      <c r="N20" t="s">
         <v>342</v>
       </c>
-      <c r="K20" t="s">
+      <c r="O20" t="s">
         <v>343</v>
       </c>
-      <c r="L20" t="s">
+      <c r="P20" t="s">
         <v>344</v>
       </c>
-      <c r="M20" t="s">
-        <v>85</v>
-      </c>
-      <c r="N20" t="s">
+      <c r="Q20" t="s">
         <v>345</v>
       </c>
-      <c r="O20" t="s">
+      <c r="R20" t="s">
         <v>346</v>
       </c>
-      <c r="P20" t="s">
+      <c r="S20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>347</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>348</v>
-      </c>
-      <c r="R20" t="s">
-        <v>349</v>
-      </c>
-      <c r="S20" t="s">
-        <v>350</v>
-      </c>
-      <c r="T20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>351</v>
       </c>
       <c r="B21">
         <v>32</v>
@@ -3863,60 +3790,57 @@
         <v>61.6</v>
       </c>
       <c r="D21" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E21" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F21" t="s">
+        <v>349</v>
+      </c>
+      <c r="G21" t="s">
+        <v>350</v>
+      </c>
+      <c r="H21" t="s">
+        <v>351</v>
+      </c>
+      <c r="I21" t="s">
         <v>353</v>
       </c>
-      <c r="G21" t="s">
+      <c r="J21" t="s">
+        <v>62</v>
+      </c>
+      <c r="K21" t="s">
         <v>354</v>
       </c>
-      <c r="H21" t="s">
+      <c r="L21" t="s">
         <v>355</v>
       </c>
-      <c r="I21" t="s">
+      <c r="M21" t="s">
+        <v>356</v>
+      </c>
+      <c r="N21" t="s">
         <v>357</v>
       </c>
-      <c r="J21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="O21" t="s">
         <v>358</v>
       </c>
-      <c r="L21" t="s">
+      <c r="P21" t="s">
         <v>359</v>
       </c>
-      <c r="M21" t="s">
-        <v>85</v>
-      </c>
-      <c r="N21" t="s">
+      <c r="Q21" t="s">
         <v>360</v>
       </c>
-      <c r="O21" t="s">
+      <c r="R21" t="s">
         <v>361</v>
       </c>
-      <c r="P21" t="s">
+      <c r="S21" t="s">
         <v>362</v>
       </c>
-      <c r="Q21" t="s">
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>363</v>
-      </c>
-      <c r="R21" t="s">
-        <v>364</v>
-      </c>
-      <c r="S21" t="s">
-        <v>365</v>
-      </c>
-      <c r="T21" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>367</v>
       </c>
       <c r="B22">
         <v>35</v>
@@ -3925,60 +3849,57 @@
         <v>60.8</v>
       </c>
       <c r="D22" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E22" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F22" t="s">
+        <v>365</v>
+      </c>
+      <c r="G22" t="s">
+        <v>366</v>
+      </c>
+      <c r="H22" t="s">
+        <v>367</v>
+      </c>
+      <c r="I22" t="s">
         <v>369</v>
       </c>
-      <c r="G22" t="s">
+      <c r="J22" t="s">
+        <v>166</v>
+      </c>
+      <c r="K22" t="s">
         <v>370</v>
       </c>
-      <c r="H22" t="s">
+      <c r="L22" t="s">
         <v>371</v>
       </c>
-      <c r="I22" t="s">
+      <c r="M22" t="s">
+        <v>372</v>
+      </c>
+      <c r="N22" t="s">
         <v>373</v>
       </c>
-      <c r="J22" t="s">
-        <v>170</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="O22" t="s">
         <v>374</v>
       </c>
-      <c r="L22" t="s">
+      <c r="P22" t="s">
         <v>375</v>
       </c>
-      <c r="M22" t="s">
-        <v>85</v>
-      </c>
-      <c r="N22" t="s">
+      <c r="Q22" t="s">
         <v>376</v>
       </c>
-      <c r="O22" t="s">
+      <c r="R22" t="s">
         <v>377</v>
       </c>
-      <c r="P22" t="s">
+      <c r="S22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>378</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>379</v>
-      </c>
-      <c r="R22" t="s">
-        <v>380</v>
-      </c>
-      <c r="S22" t="s">
-        <v>381</v>
-      </c>
-      <c r="T22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>382</v>
       </c>
       <c r="B23">
         <v>17</v>
@@ -3987,60 +3908,57 @@
         <v>77.099999999999994</v>
       </c>
       <c r="D23" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E23" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F23" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="G23" t="s">
+        <v>381</v>
+      </c>
+      <c r="H23" t="s">
+        <v>382</v>
+      </c>
+      <c r="I23" t="s">
         <v>385</v>
       </c>
-      <c r="H23" t="s">
+      <c r="J23" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" t="s">
         <v>386</v>
       </c>
-      <c r="I23" t="s">
+      <c r="L23" t="s">
+        <v>387</v>
+      </c>
+      <c r="M23" t="s">
+        <v>388</v>
+      </c>
+      <c r="N23" t="s">
         <v>389</v>
       </c>
-      <c r="J23" t="s">
-        <v>30</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="O23" t="s">
         <v>390</v>
       </c>
-      <c r="L23" t="s">
+      <c r="P23" t="s">
         <v>391</v>
       </c>
-      <c r="M23" t="s">
-        <v>29</v>
-      </c>
-      <c r="N23" t="s">
+      <c r="Q23" t="s">
         <v>392</v>
       </c>
-      <c r="O23" t="s">
+      <c r="R23" t="s">
         <v>393</v>
       </c>
-      <c r="P23" t="s">
+      <c r="S23" t="s">
         <v>394</v>
       </c>
-      <c r="Q23" t="s">
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>395</v>
-      </c>
-      <c r="R23" t="s">
-        <v>396</v>
-      </c>
-      <c r="S23" t="s">
-        <v>397</v>
-      </c>
-      <c r="T23" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>399</v>
       </c>
       <c r="B24">
         <v>20</v>
@@ -4049,60 +3967,57 @@
         <v>76.8</v>
       </c>
       <c r="D24" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E24" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F24" t="s">
+        <v>397</v>
+      </c>
+      <c r="G24" t="s">
+        <v>398</v>
+      </c>
+      <c r="H24" t="s">
+        <v>399</v>
+      </c>
+      <c r="I24" t="s">
         <v>401</v>
       </c>
-      <c r="G24" t="s">
+      <c r="J24" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" t="s">
         <v>402</v>
       </c>
-      <c r="H24" t="s">
+      <c r="L24" t="s">
         <v>403</v>
       </c>
-      <c r="I24" t="s">
+      <c r="M24" t="s">
+        <v>404</v>
+      </c>
+      <c r="N24" t="s">
         <v>405</v>
       </c>
-      <c r="J24" t="s">
-        <v>30</v>
-      </c>
-      <c r="K24" t="s">
+      <c r="O24" t="s">
         <v>406</v>
       </c>
-      <c r="L24" t="s">
+      <c r="P24" t="s">
         <v>407</v>
       </c>
-      <c r="M24" t="s">
-        <v>67</v>
-      </c>
-      <c r="N24" t="s">
+      <c r="Q24" t="s">
         <v>408</v>
       </c>
-      <c r="O24" t="s">
+      <c r="R24" t="s">
         <v>409</v>
       </c>
-      <c r="P24" t="s">
+      <c r="S24" t="s">
         <v>410</v>
       </c>
-      <c r="Q24" t="s">
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>411</v>
-      </c>
-      <c r="R24" t="s">
-        <v>412</v>
-      </c>
-      <c r="S24" t="s">
-        <v>413</v>
-      </c>
-      <c r="T24" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>415</v>
       </c>
       <c r="B25">
         <v>23</v>
@@ -4111,60 +4026,57 @@
         <v>76.400000000000006</v>
       </c>
       <c r="D25" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F25" t="s">
+        <v>413</v>
+      </c>
+      <c r="G25" t="s">
+        <v>414</v>
+      </c>
+      <c r="H25" t="s">
+        <v>415</v>
+      </c>
+      <c r="I25" t="s">
         <v>417</v>
       </c>
-      <c r="G25" t="s">
+      <c r="J25" t="s">
         <v>418</v>
       </c>
-      <c r="H25" t="s">
+      <c r="K25" t="s">
         <v>419</v>
       </c>
-      <c r="I25" t="s">
+      <c r="L25" t="s">
+        <v>420</v>
+      </c>
+      <c r="M25" t="s">
         <v>421</v>
       </c>
-      <c r="J25" t="s">
+      <c r="N25" t="s">
         <v>422</v>
       </c>
-      <c r="K25" t="s">
+      <c r="O25" t="s">
+        <v>261</v>
+      </c>
+      <c r="P25" t="s">
         <v>423</v>
       </c>
-      <c r="L25" t="s">
+      <c r="Q25" t="s">
         <v>424</v>
       </c>
-      <c r="M25" t="s">
-        <v>67</v>
-      </c>
-      <c r="N25" t="s">
+      <c r="R25" t="s">
         <v>425</v>
       </c>
-      <c r="O25" t="s">
+      <c r="S25" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>426</v>
-      </c>
-      <c r="P25" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>427</v>
-      </c>
-      <c r="R25" t="s">
-        <v>428</v>
-      </c>
-      <c r="S25" t="s">
-        <v>429</v>
-      </c>
-      <c r="T25" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>430</v>
       </c>
       <c r="B26">
         <v>26</v>
@@ -4173,60 +4085,57 @@
         <v>76.099999999999994</v>
       </c>
       <c r="D26" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E26" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F26" t="s">
+        <v>428</v>
+      </c>
+      <c r="G26" t="s">
+        <v>429</v>
+      </c>
+      <c r="H26" t="s">
+        <v>430</v>
+      </c>
+      <c r="I26" t="s">
         <v>432</v>
       </c>
-      <c r="G26" t="s">
+      <c r="J26" t="s">
         <v>433</v>
       </c>
-      <c r="H26" t="s">
+      <c r="K26" t="s">
         <v>434</v>
       </c>
-      <c r="I26" t="s">
+      <c r="L26" t="s">
+        <v>435</v>
+      </c>
+      <c r="M26" t="s">
         <v>436</v>
       </c>
-      <c r="J26" t="s">
+      <c r="N26" t="s">
         <v>437</v>
       </c>
-      <c r="K26" t="s">
+      <c r="O26" t="s">
         <v>438</v>
       </c>
-      <c r="L26" t="s">
+      <c r="P26" t="s">
         <v>439</v>
       </c>
-      <c r="M26" t="s">
-        <v>85</v>
-      </c>
-      <c r="N26" t="s">
+      <c r="Q26" t="s">
         <v>440</v>
       </c>
-      <c r="O26" t="s">
+      <c r="R26" t="s">
         <v>441</v>
       </c>
-      <c r="P26" t="s">
+      <c r="S26" t="s">
         <v>442</v>
       </c>
-      <c r="Q26" t="s">
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>443</v>
-      </c>
-      <c r="R26" t="s">
-        <v>444</v>
-      </c>
-      <c r="S26" t="s">
-        <v>445</v>
-      </c>
-      <c r="T26" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>447</v>
       </c>
       <c r="B27">
         <v>29</v>
@@ -4235,60 +4144,57 @@
         <v>75.599999999999994</v>
       </c>
       <c r="D27" t="s">
+        <v>444</v>
+      </c>
+      <c r="E27" t="s">
+        <v>199</v>
+      </c>
+      <c r="F27" t="s">
+        <v>445</v>
+      </c>
+      <c r="G27" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" t="s">
+        <v>321</v>
+      </c>
+      <c r="I27" t="s">
+        <v>447</v>
+      </c>
+      <c r="J27" t="s">
         <v>448</v>
       </c>
-      <c r="E27" t="s">
-        <v>203</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="K27" t="s">
         <v>449</v>
       </c>
-      <c r="G27" t="s">
-        <v>42</v>
-      </c>
-      <c r="H27" t="s">
-        <v>325</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="L27" t="s">
+        <v>450</v>
+      </c>
+      <c r="M27" t="s">
         <v>451</v>
       </c>
-      <c r="J27" t="s">
+      <c r="N27" t="s">
         <v>452</v>
       </c>
-      <c r="K27" t="s">
+      <c r="O27" t="s">
         <v>453</v>
       </c>
-      <c r="L27" t="s">
+      <c r="P27" t="s">
         <v>454</v>
       </c>
-      <c r="M27" t="s">
-        <v>85</v>
-      </c>
-      <c r="N27" t="s">
+      <c r="Q27" t="s">
         <v>455</v>
       </c>
-      <c r="O27" t="s">
+      <c r="R27" t="s">
         <v>456</v>
       </c>
-      <c r="P27" t="s">
+      <c r="S27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>457</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>458</v>
-      </c>
-      <c r="R27" t="s">
-        <v>459</v>
-      </c>
-      <c r="S27" t="s">
-        <v>460</v>
-      </c>
-      <c r="T27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>461</v>
       </c>
       <c r="B28">
         <v>32</v>
@@ -4297,60 +4203,57 @@
         <v>75.099999999999994</v>
       </c>
       <c r="D28" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="E28" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F28" t="s">
+        <v>459</v>
+      </c>
+      <c r="G28" t="s">
+        <v>460</v>
+      </c>
+      <c r="H28" t="s">
+        <v>461</v>
+      </c>
+      <c r="I28" t="s">
         <v>463</v>
       </c>
-      <c r="G28" t="s">
+      <c r="J28" t="s">
         <v>464</v>
       </c>
-      <c r="H28" t="s">
+      <c r="K28" t="s">
         <v>465</v>
       </c>
-      <c r="I28" t="s">
+      <c r="L28" t="s">
+        <v>466</v>
+      </c>
+      <c r="M28" t="s">
         <v>467</v>
       </c>
-      <c r="J28" t="s">
+      <c r="N28" t="s">
         <v>468</v>
       </c>
-      <c r="K28" t="s">
+      <c r="O28" t="s">
         <v>469</v>
       </c>
-      <c r="L28" t="s">
+      <c r="P28" t="s">
         <v>470</v>
       </c>
-      <c r="M28" t="s">
-        <v>85</v>
-      </c>
-      <c r="N28" t="s">
+      <c r="Q28" t="s">
         <v>471</v>
       </c>
-      <c r="O28" t="s">
+      <c r="R28" t="s">
         <v>472</v>
       </c>
-      <c r="P28" t="s">
+      <c r="S28" t="s">
         <v>473</v>
       </c>
-      <c r="Q28" t="s">
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>474</v>
-      </c>
-      <c r="R28" t="s">
-        <v>475</v>
-      </c>
-      <c r="S28" t="s">
-        <v>476</v>
-      </c>
-      <c r="T28" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>478</v>
       </c>
       <c r="B29">
         <v>35</v>
@@ -4359,60 +4262,57 @@
         <v>74.599999999999994</v>
       </c>
       <c r="D29" t="s">
+        <v>475</v>
+      </c>
+      <c r="E29" t="s">
+        <v>476</v>
+      </c>
+      <c r="F29" t="s">
+        <v>477</v>
+      </c>
+      <c r="G29" t="s">
+        <v>478</v>
+      </c>
+      <c r="H29" t="s">
         <v>479</v>
       </c>
-      <c r="E29" t="s">
-        <v>480</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="I29" t="s">
         <v>481</v>
       </c>
-      <c r="G29" t="s">
+      <c r="J29" t="s">
+        <v>418</v>
+      </c>
+      <c r="K29" t="s">
         <v>482</v>
       </c>
-      <c r="H29" t="s">
+      <c r="L29" t="s">
         <v>483</v>
       </c>
-      <c r="I29" t="s">
+      <c r="M29" t="s">
+        <v>484</v>
+      </c>
+      <c r="N29" t="s">
         <v>485</v>
       </c>
-      <c r="J29" t="s">
-        <v>422</v>
-      </c>
-      <c r="K29" t="s">
+      <c r="O29" t="s">
         <v>486</v>
       </c>
-      <c r="L29" t="s">
+      <c r="P29" t="s">
         <v>487</v>
       </c>
-      <c r="M29" t="s">
-        <v>85</v>
-      </c>
-      <c r="N29" t="s">
+      <c r="Q29" t="s">
         <v>488</v>
       </c>
-      <c r="O29" t="s">
+      <c r="R29" t="s">
         <v>489</v>
       </c>
-      <c r="P29" t="s">
+      <c r="S29" t="s">
         <v>490</v>
       </c>
-      <c r="Q29" t="s">
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>491</v>
-      </c>
-      <c r="R29" t="s">
-        <v>492</v>
-      </c>
-      <c r="S29" t="s">
-        <v>493</v>
-      </c>
-      <c r="T29" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>495</v>
       </c>
       <c r="B30">
         <v>17</v>
@@ -4421,60 +4321,57 @@
         <v>67.099999999999994</v>
       </c>
       <c r="D30" t="s">
+        <v>492</v>
+      </c>
+      <c r="E30" t="s">
+        <v>493</v>
+      </c>
+      <c r="F30" t="s">
+        <v>494</v>
+      </c>
+      <c r="G30" t="s">
+        <v>495</v>
+      </c>
+      <c r="H30" t="s">
         <v>496</v>
       </c>
-      <c r="E30" t="s">
-        <v>497</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="I30" t="s">
         <v>498</v>
       </c>
-      <c r="G30" t="s">
+      <c r="J30" t="s">
         <v>499</v>
       </c>
-      <c r="H30" t="s">
+      <c r="K30" t="s">
         <v>500</v>
       </c>
-      <c r="I30" t="s">
+      <c r="L30" t="s">
+        <v>501</v>
+      </c>
+      <c r="M30" t="s">
+        <v>31</v>
+      </c>
+      <c r="N30" t="s">
         <v>502</v>
       </c>
-      <c r="J30" t="s">
+      <c r="O30" t="s">
         <v>503</v>
       </c>
-      <c r="K30" t="s">
+      <c r="P30" t="s">
         <v>504</v>
       </c>
-      <c r="L30" t="s">
+      <c r="Q30" t="s">
         <v>505</v>
       </c>
-      <c r="M30" t="s">
-        <v>29</v>
-      </c>
-      <c r="N30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O30" t="s">
+      <c r="R30" t="s">
         <v>506</v>
       </c>
-      <c r="P30" t="s">
+      <c r="S30" t="s">
         <v>507</v>
       </c>
-      <c r="Q30" t="s">
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>508</v>
-      </c>
-      <c r="R30" t="s">
-        <v>509</v>
-      </c>
-      <c r="S30" t="s">
-        <v>510</v>
-      </c>
-      <c r="T30" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>512</v>
       </c>
       <c r="B31">
         <v>20</v>
@@ -4483,60 +4380,57 @@
         <v>66.3</v>
       </c>
       <c r="D31" t="s">
+        <v>509</v>
+      </c>
+      <c r="E31" t="s">
+        <v>510</v>
+      </c>
+      <c r="F31" t="s">
+        <v>511</v>
+      </c>
+      <c r="G31" t="s">
+        <v>512</v>
+      </c>
+      <c r="H31" t="s">
         <v>513</v>
       </c>
-      <c r="E31" t="s">
-        <v>514</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="I31" t="s">
         <v>515</v>
       </c>
-      <c r="G31" t="s">
+      <c r="J31" t="s">
+        <v>448</v>
+      </c>
+      <c r="K31" t="s">
         <v>516</v>
       </c>
-      <c r="H31" t="s">
+      <c r="L31" t="s">
         <v>517</v>
       </c>
-      <c r="I31" t="s">
+      <c r="M31" t="s">
+        <v>518</v>
+      </c>
+      <c r="N31" t="s">
         <v>519</v>
       </c>
-      <c r="J31" t="s">
-        <v>452</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="O31" t="s">
         <v>520</v>
       </c>
-      <c r="L31" t="s">
+      <c r="P31" t="s">
         <v>521</v>
       </c>
-      <c r="M31" t="s">
-        <v>67</v>
-      </c>
-      <c r="N31" t="s">
+      <c r="Q31" t="s">
         <v>522</v>
       </c>
-      <c r="O31" t="s">
+      <c r="R31" t="s">
         <v>523</v>
       </c>
-      <c r="P31" t="s">
+      <c r="S31" t="s">
         <v>524</v>
       </c>
-      <c r="Q31" t="s">
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>525</v>
-      </c>
-      <c r="R31" t="s">
-        <v>526</v>
-      </c>
-      <c r="S31" t="s">
-        <v>527</v>
-      </c>
-      <c r="T31" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>529</v>
       </c>
       <c r="B32">
         <v>23</v>
@@ -4545,60 +4439,57 @@
         <v>65.8</v>
       </c>
       <c r="D32" t="s">
+        <v>526</v>
+      </c>
+      <c r="E32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F32" t="s">
+        <v>527</v>
+      </c>
+      <c r="G32" t="s">
+        <v>334</v>
+      </c>
+      <c r="H32" t="s">
+        <v>528</v>
+      </c>
+      <c r="I32" t="s">
         <v>530</v>
       </c>
-      <c r="E32" t="s">
-        <v>501</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="J32" t="s">
         <v>531</v>
       </c>
-      <c r="G32" t="s">
-        <v>338</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="K32" t="s">
         <v>532</v>
       </c>
-      <c r="I32" t="s">
+      <c r="L32" t="s">
+        <v>533</v>
+      </c>
+      <c r="M32" t="s">
         <v>534</v>
       </c>
-      <c r="J32" t="s">
+      <c r="N32" t="s">
         <v>535</v>
       </c>
-      <c r="K32" t="s">
+      <c r="O32" t="s">
         <v>536</v>
       </c>
-      <c r="L32" t="s">
+      <c r="P32" t="s">
         <v>537</v>
       </c>
-      <c r="M32" t="s">
-        <v>67</v>
-      </c>
-      <c r="N32" t="s">
+      <c r="Q32" t="s">
         <v>538</v>
       </c>
-      <c r="O32" t="s">
+      <c r="R32" t="s">
         <v>539</v>
       </c>
-      <c r="P32" t="s">
+      <c r="S32" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>540</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>541</v>
-      </c>
-      <c r="R32" t="s">
-        <v>542</v>
-      </c>
-      <c r="S32" t="s">
-        <v>543</v>
-      </c>
-      <c r="T32" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>544</v>
       </c>
       <c r="B33">
         <v>26</v>
@@ -4607,60 +4498,57 @@
         <v>65.900000000000006</v>
       </c>
       <c r="D33" t="s">
+        <v>541</v>
+      </c>
+      <c r="E33" t="s">
+        <v>542</v>
+      </c>
+      <c r="F33" t="s">
+        <v>543</v>
+      </c>
+      <c r="G33" t="s">
+        <v>544</v>
+      </c>
+      <c r="H33" t="s">
         <v>545</v>
       </c>
-      <c r="E33" t="s">
-        <v>546</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="I33" t="s">
         <v>547</v>
       </c>
-      <c r="G33" t="s">
+      <c r="J33" t="s">
+        <v>149</v>
+      </c>
+      <c r="K33" t="s">
         <v>548</v>
       </c>
-      <c r="H33" t="s">
+      <c r="L33" t="s">
         <v>549</v>
       </c>
-      <c r="I33" t="s">
+      <c r="M33" t="s">
+        <v>550</v>
+      </c>
+      <c r="N33" t="s">
         <v>551</v>
       </c>
-      <c r="J33" t="s">
-        <v>153</v>
-      </c>
-      <c r="K33" t="s">
+      <c r="O33" t="s">
         <v>552</v>
       </c>
-      <c r="L33" t="s">
+      <c r="P33" t="s">
         <v>553</v>
       </c>
-      <c r="M33" t="s">
-        <v>67</v>
-      </c>
-      <c r="N33" t="s">
+      <c r="Q33" t="s">
         <v>554</v>
       </c>
-      <c r="O33" t="s">
+      <c r="R33" t="s">
         <v>555</v>
       </c>
-      <c r="P33" t="s">
+      <c r="S33" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>556</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>557</v>
-      </c>
-      <c r="R33" t="s">
-        <v>558</v>
-      </c>
-      <c r="S33" t="s">
-        <v>559</v>
-      </c>
-      <c r="T33" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>560</v>
       </c>
       <c r="B34">
         <v>29</v>
@@ -4669,60 +4557,57 @@
         <v>65.8</v>
       </c>
       <c r="D34" t="s">
+        <v>557</v>
+      </c>
+      <c r="E34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" t="s">
+        <v>253</v>
+      </c>
+      <c r="G34" t="s">
+        <v>558</v>
+      </c>
+      <c r="H34" t="s">
+        <v>559</v>
+      </c>
+      <c r="I34" t="s">
         <v>561</v>
       </c>
-      <c r="E34" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" t="s">
-        <v>257</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="J34" t="s">
+        <v>499</v>
+      </c>
+      <c r="K34" t="s">
         <v>562</v>
       </c>
-      <c r="H34" t="s">
+      <c r="L34" t="s">
         <v>563</v>
       </c>
-      <c r="I34" t="s">
+      <c r="M34" t="s">
+        <v>564</v>
+      </c>
+      <c r="N34" t="s">
+        <v>309</v>
+      </c>
+      <c r="O34" t="s">
         <v>565</v>
       </c>
-      <c r="J34" t="s">
-        <v>503</v>
-      </c>
-      <c r="K34" t="s">
+      <c r="P34" t="s">
         <v>566</v>
       </c>
-      <c r="L34" t="s">
+      <c r="Q34" t="s">
         <v>567</v>
       </c>
-      <c r="M34" t="s">
-        <v>67</v>
-      </c>
-      <c r="N34" t="s">
+      <c r="R34" t="s">
         <v>568</v>
       </c>
-      <c r="O34" t="s">
-        <v>313</v>
-      </c>
-      <c r="P34" t="s">
+      <c r="S34" t="s">
         <v>569</v>
       </c>
-      <c r="Q34" t="s">
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>570</v>
-      </c>
-      <c r="R34" t="s">
-        <v>571</v>
-      </c>
-      <c r="S34" t="s">
-        <v>572</v>
-      </c>
-      <c r="T34" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>574</v>
       </c>
       <c r="B35">
         <v>32</v>
@@ -4731,60 +4616,57 @@
         <v>65.3</v>
       </c>
       <c r="D35" t="s">
+        <v>571</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" t="s">
+        <v>572</v>
+      </c>
+      <c r="G35" t="s">
+        <v>573</v>
+      </c>
+      <c r="H35" t="s">
+        <v>574</v>
+      </c>
+      <c r="I35" t="s">
         <v>575</v>
       </c>
-      <c r="E35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="J35" t="s">
+        <v>448</v>
+      </c>
+      <c r="K35" t="s">
         <v>576</v>
       </c>
-      <c r="G35" t="s">
+      <c r="L35" t="s">
         <v>577</v>
       </c>
-      <c r="H35" t="s">
+      <c r="M35" t="s">
         <v>578</v>
       </c>
-      <c r="I35" t="s">
+      <c r="N35" t="s">
         <v>579</v>
       </c>
-      <c r="J35" t="s">
-        <v>452</v>
-      </c>
-      <c r="K35" t="s">
+      <c r="O35" t="s">
         <v>580</v>
       </c>
-      <c r="L35" t="s">
+      <c r="P35" t="s">
         <v>581</v>
       </c>
-      <c r="M35" t="s">
-        <v>85</v>
-      </c>
-      <c r="N35" t="s">
+      <c r="Q35" t="s">
         <v>582</v>
       </c>
-      <c r="O35" t="s">
+      <c r="R35" t="s">
         <v>583</v>
       </c>
-      <c r="P35" t="s">
+      <c r="S35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>584</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>585</v>
-      </c>
-      <c r="R35" t="s">
-        <v>586</v>
-      </c>
-      <c r="S35" t="s">
-        <v>587</v>
-      </c>
-      <c r="T35" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>588</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -4793,60 +4675,57 @@
         <v>65.400000000000006</v>
       </c>
       <c r="D36" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="E36" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F36" t="s">
+        <v>586</v>
+      </c>
+      <c r="G36" t="s">
+        <v>587</v>
+      </c>
+      <c r="H36" t="s">
+        <v>588</v>
+      </c>
+      <c r="I36" t="s">
         <v>590</v>
       </c>
-      <c r="G36" t="s">
+      <c r="J36" t="s">
         <v>591</v>
       </c>
-      <c r="H36" t="s">
+      <c r="K36" t="s">
         <v>592</v>
       </c>
-      <c r="I36" t="s">
+      <c r="L36" t="s">
+        <v>593</v>
+      </c>
+      <c r="M36" t="s">
         <v>594</v>
       </c>
-      <c r="J36" t="s">
+      <c r="N36" t="s">
         <v>595</v>
       </c>
-      <c r="K36" t="s">
+      <c r="O36" t="s">
         <v>596</v>
       </c>
-      <c r="L36" t="s">
+      <c r="P36" t="s">
         <v>597</v>
       </c>
-      <c r="M36" t="s">
-        <v>85</v>
-      </c>
-      <c r="N36" t="s">
+      <c r="Q36" t="s">
         <v>598</v>
       </c>
-      <c r="O36" t="s">
+      <c r="R36" t="s">
         <v>599</v>
       </c>
-      <c r="P36" t="s">
+      <c r="S36" t="s">
         <v>600</v>
       </c>
-      <c r="Q36" t="s">
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>601</v>
-      </c>
-      <c r="R36" t="s">
-        <v>602</v>
-      </c>
-      <c r="S36" t="s">
-        <v>603</v>
-      </c>
-      <c r="T36" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>605</v>
       </c>
       <c r="B37">
         <v>17</v>
@@ -4855,60 +4734,57 @@
         <v>82.9</v>
       </c>
       <c r="D37" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="E37" t="s">
+        <v>603</v>
+      </c>
+      <c r="F37" t="s">
+        <v>604</v>
+      </c>
+      <c r="G37" t="s">
+        <v>219</v>
+      </c>
+      <c r="H37" t="s">
+        <v>605</v>
+      </c>
+      <c r="I37" t="s">
         <v>607</v>
       </c>
-      <c r="F37" t="s">
+      <c r="J37" t="s">
         <v>608</v>
       </c>
-      <c r="G37" t="s">
-        <v>223</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="K37" t="s">
         <v>609</v>
       </c>
-      <c r="I37" t="s">
+      <c r="L37" t="s">
+        <v>610</v>
+      </c>
+      <c r="M37" t="s">
         <v>611</v>
       </c>
-      <c r="J37" t="s">
+      <c r="N37" t="s">
         <v>612</v>
       </c>
-      <c r="K37" t="s">
+      <c r="O37" t="s">
         <v>613</v>
       </c>
-      <c r="L37" t="s">
+      <c r="P37" t="s">
         <v>614</v>
       </c>
-      <c r="M37" t="s">
-        <v>29</v>
-      </c>
-      <c r="N37" t="s">
+      <c r="Q37" t="s">
         <v>615</v>
       </c>
-      <c r="O37" t="s">
+      <c r="R37" t="s">
         <v>616</v>
       </c>
-      <c r="P37" t="s">
+      <c r="S37" t="s">
         <v>617</v>
       </c>
-      <c r="Q37" t="s">
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>618</v>
-      </c>
-      <c r="R37" t="s">
-        <v>619</v>
-      </c>
-      <c r="S37" t="s">
-        <v>620</v>
-      </c>
-      <c r="T37" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>622</v>
       </c>
       <c r="B38">
         <v>20</v>
@@ -4917,60 +4793,57 @@
         <v>82.2</v>
       </c>
       <c r="D38" t="s">
+        <v>619</v>
+      </c>
+      <c r="E38" t="s">
+        <v>603</v>
+      </c>
+      <c r="F38" t="s">
+        <v>620</v>
+      </c>
+      <c r="G38" t="s">
+        <v>573</v>
+      </c>
+      <c r="H38" t="s">
+        <v>621</v>
+      </c>
+      <c r="I38" t="s">
         <v>623</v>
       </c>
-      <c r="E38" t="s">
-        <v>607</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="J38" t="s">
         <v>624</v>
       </c>
-      <c r="G38" t="s">
-        <v>577</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="K38" t="s">
         <v>625</v>
       </c>
-      <c r="I38" t="s">
+      <c r="L38" t="s">
+        <v>242</v>
+      </c>
+      <c r="M38" t="s">
+        <v>626</v>
+      </c>
+      <c r="N38" t="s">
         <v>627</v>
       </c>
-      <c r="J38" t="s">
+      <c r="O38" t="s">
         <v>628</v>
       </c>
-      <c r="K38" t="s">
+      <c r="P38" t="s">
         <v>629</v>
       </c>
-      <c r="L38" t="s">
-        <v>246</v>
-      </c>
-      <c r="M38" t="s">
-        <v>29</v>
-      </c>
-      <c r="N38" t="s">
+      <c r="Q38" t="s">
         <v>630</v>
       </c>
-      <c r="O38" t="s">
+      <c r="R38" t="s">
         <v>631</v>
       </c>
-      <c r="P38" t="s">
+      <c r="S38" t="s">
         <v>632</v>
       </c>
-      <c r="Q38" t="s">
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>633</v>
-      </c>
-      <c r="R38" t="s">
-        <v>634</v>
-      </c>
-      <c r="S38" t="s">
-        <v>635</v>
-      </c>
-      <c r="T38" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>637</v>
       </c>
       <c r="B39">
         <v>23</v>
@@ -4979,60 +4852,57 @@
         <v>81.599999999999994</v>
       </c>
       <c r="D39" t="s">
+        <v>634</v>
+      </c>
+      <c r="E39" t="s">
+        <v>635</v>
+      </c>
+      <c r="F39" t="s">
+        <v>636</v>
+      </c>
+      <c r="G39" t="s">
+        <v>637</v>
+      </c>
+      <c r="H39" t="s">
         <v>638</v>
       </c>
-      <c r="E39" t="s">
-        <v>639</v>
-      </c>
-      <c r="F39" t="s">
-        <v>640</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="I39" t="s">
         <v>641</v>
       </c>
-      <c r="H39" t="s">
+      <c r="J39" t="s">
+        <v>464</v>
+      </c>
+      <c r="K39" t="s">
         <v>642</v>
       </c>
-      <c r="I39" t="s">
+      <c r="L39" t="s">
+        <v>643</v>
+      </c>
+      <c r="M39" t="s">
+        <v>644</v>
+      </c>
+      <c r="N39" t="s">
+        <v>285</v>
+      </c>
+      <c r="O39" t="s">
+        <v>101</v>
+      </c>
+      <c r="P39" t="s">
         <v>645</v>
       </c>
-      <c r="J39" t="s">
-        <v>468</v>
-      </c>
-      <c r="K39" t="s">
+      <c r="Q39" t="s">
         <v>646</v>
       </c>
-      <c r="L39" t="s">
+      <c r="R39" t="s">
         <v>647</v>
       </c>
-      <c r="M39" t="s">
-        <v>67</v>
-      </c>
-      <c r="N39" t="s">
+      <c r="S39" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>648</v>
-      </c>
-      <c r="O39" t="s">
-        <v>289</v>
-      </c>
-      <c r="P39" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>649</v>
-      </c>
-      <c r="R39" t="s">
-        <v>650</v>
-      </c>
-      <c r="S39" t="s">
-        <v>651</v>
-      </c>
-      <c r="T39" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>652</v>
       </c>
       <c r="B40">
         <v>26</v>
@@ -5041,60 +4911,57 @@
         <v>81.5</v>
       </c>
       <c r="D40" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="E40" t="s">
+        <v>650</v>
+      </c>
+      <c r="F40" t="s">
+        <v>651</v>
+      </c>
+      <c r="G40" t="s">
+        <v>235</v>
+      </c>
+      <c r="H40" t="s">
+        <v>652</v>
+      </c>
+      <c r="I40" t="s">
         <v>654</v>
       </c>
-      <c r="F40" t="s">
+      <c r="J40" t="s">
         <v>655</v>
       </c>
-      <c r="G40" t="s">
-        <v>239</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="K40" t="s">
         <v>656</v>
       </c>
-      <c r="I40" t="s">
+      <c r="L40" t="s">
+        <v>657</v>
+      </c>
+      <c r="M40" t="s">
         <v>658</v>
       </c>
-      <c r="J40" t="s">
+      <c r="N40" t="s">
         <v>659</v>
       </c>
-      <c r="K40" t="s">
+      <c r="O40" t="s">
         <v>660</v>
       </c>
-      <c r="L40" t="s">
+      <c r="P40" t="s">
         <v>661</v>
       </c>
-      <c r="M40" t="s">
-        <v>67</v>
-      </c>
-      <c r="N40" t="s">
+      <c r="Q40" t="s">
         <v>662</v>
       </c>
-      <c r="O40" t="s">
+      <c r="R40" t="s">
         <v>663</v>
       </c>
-      <c r="P40" t="s">
+      <c r="S40" t="s">
         <v>664</v>
       </c>
-      <c r="Q40" t="s">
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>665</v>
-      </c>
-      <c r="R40" t="s">
-        <v>666</v>
-      </c>
-      <c r="S40" t="s">
-        <v>667</v>
-      </c>
-      <c r="T40" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>669</v>
       </c>
       <c r="B41">
         <v>29</v>
@@ -5103,60 +4970,57 @@
         <v>80.8</v>
       </c>
       <c r="D41" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E41" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="F41" t="s">
+        <v>666</v>
+      </c>
+      <c r="G41" t="s">
+        <v>667</v>
+      </c>
+      <c r="H41" t="s">
+        <v>668</v>
+      </c>
+      <c r="I41" t="s">
         <v>670</v>
       </c>
-      <c r="G41" t="s">
+      <c r="J41" t="s">
+        <v>28</v>
+      </c>
+      <c r="K41" t="s">
         <v>671</v>
       </c>
-      <c r="H41" t="s">
+      <c r="L41" t="s">
         <v>672</v>
       </c>
-      <c r="I41" t="s">
+      <c r="M41" t="s">
+        <v>673</v>
+      </c>
+      <c r="N41" t="s">
         <v>674</v>
       </c>
-      <c r="J41" t="s">
-        <v>30</v>
-      </c>
-      <c r="K41" t="s">
+      <c r="O41" t="s">
         <v>675</v>
       </c>
-      <c r="L41" t="s">
+      <c r="P41" t="s">
         <v>676</v>
       </c>
-      <c r="M41" t="s">
-        <v>67</v>
-      </c>
-      <c r="N41" t="s">
+      <c r="Q41" t="s">
         <v>677</v>
       </c>
-      <c r="O41" t="s">
+      <c r="R41" t="s">
         <v>678</v>
       </c>
-      <c r="P41" t="s">
+      <c r="S41" t="s">
         <v>679</v>
       </c>
-      <c r="Q41" t="s">
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>680</v>
-      </c>
-      <c r="R41" t="s">
-        <v>681</v>
-      </c>
-      <c r="S41" t="s">
-        <v>682</v>
-      </c>
-      <c r="T41" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>684</v>
       </c>
       <c r="B42">
         <v>32</v>
@@ -5165,60 +5029,57 @@
         <v>80.5</v>
       </c>
       <c r="D42" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="E42" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="F42" t="s">
+        <v>682</v>
+      </c>
+      <c r="G42" t="s">
+        <v>683</v>
+      </c>
+      <c r="H42" t="s">
+        <v>684</v>
+      </c>
+      <c r="I42" t="s">
         <v>686</v>
       </c>
-      <c r="G42" t="s">
+      <c r="J42" t="s">
+        <v>624</v>
+      </c>
+      <c r="K42" t="s">
         <v>687</v>
       </c>
-      <c r="H42" t="s">
+      <c r="L42" t="s">
         <v>688</v>
       </c>
-      <c r="I42" t="s">
+      <c r="M42" t="s">
+        <v>689</v>
+      </c>
+      <c r="N42" t="s">
         <v>690</v>
       </c>
-      <c r="J42" t="s">
-        <v>628</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="O42" t="s">
+        <v>377</v>
+      </c>
+      <c r="P42" t="s">
         <v>691</v>
       </c>
-      <c r="L42" t="s">
+      <c r="Q42" t="s">
         <v>692</v>
       </c>
-      <c r="M42" t="s">
-        <v>67</v>
-      </c>
-      <c r="N42" t="s">
+      <c r="R42" t="s">
         <v>693</v>
       </c>
-      <c r="O42" t="s">
+      <c r="S42" t="s">
         <v>694</v>
       </c>
-      <c r="P42" t="s">
-        <v>381</v>
-      </c>
-      <c r="Q42" t="s">
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>695</v>
-      </c>
-      <c r="R42" t="s">
-        <v>696</v>
-      </c>
-      <c r="S42" t="s">
-        <v>697</v>
-      </c>
-      <c r="T42" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>699</v>
       </c>
       <c r="B43">
         <v>35</v>
@@ -5227,55 +5088,52 @@
         <v>79</v>
       </c>
       <c r="D43" t="s">
+        <v>696</v>
+      </c>
+      <c r="E43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" t="s">
+        <v>697</v>
+      </c>
+      <c r="G43" t="s">
+        <v>639</v>
+      </c>
+      <c r="H43" t="s">
+        <v>698</v>
+      </c>
+      <c r="I43" t="s">
         <v>700</v>
       </c>
-      <c r="E43" t="s">
-        <v>40</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="J43" t="s">
         <v>701</v>
       </c>
-      <c r="G43" t="s">
-        <v>643</v>
-      </c>
-      <c r="H43" t="s">
+      <c r="K43" t="s">
         <v>702</v>
       </c>
-      <c r="I43" t="s">
+      <c r="L43" t="s">
+        <v>703</v>
+      </c>
+      <c r="M43" t="s">
         <v>704</v>
       </c>
-      <c r="J43" t="s">
+      <c r="N43" t="s">
         <v>705</v>
       </c>
-      <c r="K43" t="s">
+      <c r="O43" t="s">
+        <v>102</v>
+      </c>
+      <c r="P43" t="s">
+        <v>533</v>
+      </c>
+      <c r="Q43" t="s">
         <v>706</v>
       </c>
-      <c r="L43" t="s">
+      <c r="R43" t="s">
         <v>707</v>
       </c>
-      <c r="M43" t="s">
-        <v>67</v>
-      </c>
-      <c r="N43" t="s">
+      <c r="S43" t="s">
         <v>708</v>
-      </c>
-      <c r="O43" t="s">
-        <v>709</v>
-      </c>
-      <c r="P43" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>537</v>
-      </c>
-      <c r="R43" t="s">
-        <v>710</v>
-      </c>
-      <c r="S43" t="s">
-        <v>711</v>
-      </c>
-      <c r="T43" t="s">
-        <v>712</v>
       </c>
     </row>
   </sheetData>
@@ -5315,7 +5173,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <f>A2/1000</f>
@@ -5324,7 +5182,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B43" si="0">A3/1000</f>
@@ -5333,7 +5191,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
@@ -5342,7 +5200,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
@@ -5351,7 +5209,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
@@ -5360,7 +5218,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
@@ -5369,7 +5227,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
@@ -5378,7 +5236,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
@@ -5387,7 +5245,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
@@ -5396,7 +5254,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -5405,7 +5263,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
@@ -5414,7 +5272,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
@@ -5423,7 +5281,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
@@ -5432,7 +5290,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
@@ -5441,7 +5299,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -5450,7 +5308,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -5459,7 +5317,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
@@ -5468,7 +5326,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
@@ -5477,7 +5335,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
@@ -5486,7 +5344,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
@@ -5495,7 +5353,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
@@ -5504,7 +5362,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
@@ -5513,7 +5371,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
@@ -5522,7 +5380,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
@@ -5531,7 +5389,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
@@ -5540,7 +5398,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
@@ -5549,7 +5407,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
@@ -5558,7 +5416,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
@@ -5567,7 +5425,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
@@ -5576,7 +5434,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
@@ -5585,7 +5443,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
@@ -5594,7 +5452,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
@@ -5603,7 +5461,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
@@ -5612,7 +5470,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
@@ -5621,7 +5479,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
@@ -5630,7 +5488,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
@@ -5639,7 +5497,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
@@ -5648,7 +5506,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
@@ -5657,7 +5515,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
@@ -5666,7 +5524,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
@@ -5675,7 +5533,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
@@ -5684,7 +5542,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
@@ -5697,11 +5555,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="71374b10-47c5-4f6a-930a-092997f9c872" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5946,27 +5805,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="71374b10-47c5-4f6a-930a-092997f9c872" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511062F4-D224-41F7-9160-EA869FADD5C7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25DDFBE9-79B6-4FC0-A984-1A87F8215191}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="061285c2-757e-40ba-87eb-1c6076680213"/>
-    <ds:schemaRef ds:uri="71374b10-47c5-4f6a-930a-092997f9c872"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5991,9 +5840,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25DDFBE9-79B6-4FC0-A984-1A87F8215191}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{511062F4-D224-41F7-9160-EA869FADD5C7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="061285c2-757e-40ba-87eb-1c6076680213"/>
+    <ds:schemaRef ds:uri="71374b10-47c5-4f6a-930a-092997f9c872"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>